<commit_message>
Required Files for script
</commit_message>
<xml_diff>
--- a/clubdb.xlsx
+++ b/clubdb.xlsx
@@ -1,21 +1,29 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10210"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10812"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ishaanchandratreya/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/christopherkang/Documents/Columbia/DPI/ClubSwipe-Backend/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D54976F-A4B9-6F4B-962D-0CE4BE47ABA8}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{22A6C227-7D94-F549-82C9-431BED2DA432}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-20" yWindow="460" windowWidth="28800" windowHeight="16840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -2027,7 +2035,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -2038,6 +2046,12 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFFFF"/>
         <bgColor rgb="FFFFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -2061,7 +2075,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
@@ -2078,6 +2092,11 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1" applyFill="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -2398,8 +2417,8 @@
   </sheetPr>
   <dimension ref="A1:G345"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B188" sqref="B188:B340"/>
+    <sheetView tabSelected="1" topLeftCell="A284" zoomScale="143" workbookViewId="0">
+      <selection activeCell="C291" sqref="C291"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -2431,7 +2450,7 @@
       <c r="D2" s="12"/>
     </row>
     <row r="3" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B3" s="2" t="s">
+      <c r="B3" s="17" t="s">
         <v>4</v>
       </c>
       <c r="C3" s="2"/>
@@ -2515,7 +2534,7 @@
       <c r="G8" s="2"/>
     </row>
     <row r="9" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B9" s="2" t="s">
+      <c r="B9" s="15" t="s">
         <v>22</v>
       </c>
       <c r="C9" s="2"/>
@@ -2543,7 +2562,7 @@
       </c>
     </row>
     <row r="11" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B11" s="2" t="s">
+      <c r="B11" s="14" t="s">
         <v>28</v>
       </c>
       <c r="C11" s="2"/>
@@ -2633,7 +2652,7 @@
       <c r="G17" s="3"/>
     </row>
     <row r="18" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B18" s="2" t="s">
+      <c r="B18" s="14" t="s">
         <v>45</v>
       </c>
       <c r="C18" s="2"/>
@@ -2675,7 +2694,7 @@
       <c r="G20" s="2"/>
     </row>
     <row r="21" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B21" s="2" t="s">
+      <c r="B21" s="14" t="s">
         <v>54</v>
       </c>
       <c r="C21" s="2"/>
@@ -2743,7 +2762,7 @@
       </c>
     </row>
     <row r="26" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B26" s="2" t="s">
+      <c r="B26" s="14" t="s">
         <v>68</v>
       </c>
       <c r="C26" s="2"/>
@@ -3005,7 +3024,7 @@
       <c r="G44" s="2"/>
     </row>
     <row r="45" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B45" s="2" t="s">
+      <c r="B45" s="14" t="s">
         <v>122</v>
       </c>
       <c r="C45" s="2"/>
@@ -3019,7 +3038,7 @@
       </c>
     </row>
     <row r="46" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B46" s="2" t="s">
+      <c r="B46" s="14" t="s">
         <v>125</v>
       </c>
       <c r="C46" s="2"/>
@@ -3033,7 +3052,7 @@
       </c>
     </row>
     <row r="47" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B47" s="2" t="s">
+      <c r="B47" s="14" t="s">
         <v>128</v>
       </c>
       <c r="C47" s="2"/>
@@ -3045,7 +3064,7 @@
       <c r="G47" s="2"/>
     </row>
     <row r="48" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B48" s="2" t="s">
+      <c r="B48" s="14" t="s">
         <v>130</v>
       </c>
       <c r="C48" s="2"/>
@@ -3059,7 +3078,7 @@
       </c>
     </row>
     <row r="49" spans="2:7" ht="13" x14ac:dyDescent="0.15">
-      <c r="B49" s="2" t="s">
+      <c r="B49" s="14" t="s">
         <v>133</v>
       </c>
       <c r="C49" s="2"/>
@@ -3087,7 +3106,7 @@
       <c r="G50" s="2"/>
     </row>
     <row r="51" spans="2:7" ht="13" x14ac:dyDescent="0.15">
-      <c r="B51" s="2" t="s">
+      <c r="B51" s="14" t="s">
         <v>139</v>
       </c>
       <c r="C51" s="2"/>
@@ -3101,7 +3120,7 @@
       <c r="G51" s="2"/>
     </row>
     <row r="52" spans="2:7" ht="16" x14ac:dyDescent="0.2">
-      <c r="B52" s="3" t="s">
+      <c r="B52" s="15" t="s">
         <v>142</v>
       </c>
       <c r="C52" s="2"/>
@@ -3115,7 +3134,7 @@
       <c r="G52" s="2"/>
     </row>
     <row r="53" spans="2:7" ht="13" x14ac:dyDescent="0.15">
-      <c r="B53" s="3" t="s">
+      <c r="B53" s="14" t="s">
         <v>145</v>
       </c>
       <c r="C53" s="2"/>
@@ -3183,7 +3202,7 @@
       <c r="G57" s="2"/>
     </row>
     <row r="58" spans="2:7" ht="16" x14ac:dyDescent="0.2">
-      <c r="B58" s="2" t="s">
+      <c r="B58" s="14" t="s">
         <v>159</v>
       </c>
       <c r="C58" s="2"/>
@@ -3197,7 +3216,7 @@
       <c r="G58" s="2"/>
     </row>
     <row r="59" spans="2:7" ht="16" x14ac:dyDescent="0.2">
-      <c r="B59" s="2" t="s">
+      <c r="B59" s="14" t="s">
         <v>162</v>
       </c>
       <c r="C59" s="2"/>
@@ -3211,7 +3230,7 @@
       <c r="G59" s="2"/>
     </row>
     <row r="60" spans="2:7" ht="13" x14ac:dyDescent="0.15">
-      <c r="B60" s="2" t="s">
+      <c r="B60" s="14" t="s">
         <v>165</v>
       </c>
       <c r="C60" s="2"/>
@@ -3615,7 +3634,7 @@
       <c r="G88" s="2"/>
     </row>
     <row r="89" spans="2:7" ht="13" x14ac:dyDescent="0.15">
-      <c r="B89" s="2" t="s">
+      <c r="B89" s="14" t="s">
         <v>251</v>
       </c>
       <c r="C89" s="2"/>
@@ -3927,7 +3946,7 @@
       <c r="G111" s="2"/>
     </row>
     <row r="112" spans="2:7" ht="16" x14ac:dyDescent="0.2">
-      <c r="B112" s="2" t="s">
+      <c r="B112" s="14" t="s">
         <v>315</v>
       </c>
       <c r="C112" s="2"/>
@@ -4037,7 +4056,7 @@
       </c>
     </row>
     <row r="120" spans="2:7" ht="13" x14ac:dyDescent="0.15">
-      <c r="B120" s="2" t="s">
+      <c r="B120" s="14" t="s">
         <v>338</v>
       </c>
       <c r="C120" s="2"/>
@@ -4319,7 +4338,7 @@
       <c r="G140" s="3"/>
     </row>
     <row r="141" spans="2:7" ht="13" x14ac:dyDescent="0.15">
-      <c r="B141" s="2" t="s">
+      <c r="B141" s="14" t="s">
         <v>394</v>
       </c>
       <c r="C141" s="2"/>
@@ -4423,7 +4442,7 @@
       </c>
     </row>
     <row r="149" spans="2:7" ht="13" x14ac:dyDescent="0.15">
-      <c r="B149" s="2" t="s">
+      <c r="B149" s="14" t="s">
         <v>414</v>
       </c>
       <c r="C149" s="2"/>
@@ -4703,7 +4722,7 @@
       </c>
     </row>
     <row r="170" spans="2:7" ht="13" x14ac:dyDescent="0.15">
-      <c r="B170" s="2" t="s">
+      <c r="B170" s="14" t="s">
         <v>470</v>
       </c>
       <c r="C170" s="2"/>
@@ -4953,7 +4972,7 @@
       </c>
     </row>
     <row r="192" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B192" s="12" t="s">
+      <c r="B192" s="16" t="s">
         <v>517</v>
       </c>
     </row>
@@ -5048,7 +5067,7 @@
       </c>
     </row>
     <row r="211" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B211" s="12" t="s">
+      <c r="B211" s="18" t="s">
         <v>533</v>
       </c>
     </row>
@@ -5113,7 +5132,7 @@
       </c>
     </row>
     <row r="224" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B224" s="12" t="s">
+      <c r="B224" s="16" t="s">
         <v>139</v>
       </c>
     </row>
@@ -5163,7 +5182,7 @@
       </c>
     </row>
     <row r="234" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B234" s="12" t="s">
+      <c r="B234" s="16" t="s">
         <v>552</v>
       </c>
     </row>
@@ -5203,7 +5222,7 @@
       </c>
     </row>
     <row r="242" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B242" s="12" t="s">
+      <c r="B242" s="16" t="s">
         <v>560</v>
       </c>
     </row>
@@ -5283,7 +5302,7 @@
       </c>
     </row>
     <row r="258" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B258" s="12" t="s">
+      <c r="B258" s="16" t="s">
         <v>576</v>
       </c>
     </row>
@@ -5323,7 +5342,7 @@
       </c>
     </row>
     <row r="266" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B266" s="12" t="s">
+      <c r="B266" s="16" t="s">
         <v>583</v>
       </c>
     </row>
@@ -5408,7 +5427,7 @@
       </c>
     </row>
     <row r="283" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B283" s="12" t="s">
+      <c r="B283" s="16" t="s">
         <v>594</v>
       </c>
     </row>
@@ -5433,7 +5452,7 @@
       </c>
     </row>
     <row r="288" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B288" s="12" t="s">
+      <c r="B288" s="16" t="s">
         <v>597</v>
       </c>
     </row>
@@ -5528,7 +5547,7 @@
       </c>
     </row>
     <row r="307" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B307" s="12" t="s">
+      <c r="B307" s="16" t="s">
         <v>613</v>
       </c>
     </row>
@@ -5683,7 +5702,7 @@
       </c>
     </row>
     <row r="338" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B338" s="12" t="s">
+      <c r="B338" s="16" t="s">
         <v>640</v>
       </c>
     </row>

</xml_diff>